<commit_message>
Update app, config, and frontend; add admin template; update data including RMS allocations spreadsheet
</commit_message>
<xml_diff>
--- a/data/Positions.xlsx
+++ b/data/Positions.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b3db30460c098f93/Desktop/C^MA/database_app/Tables for new app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdrianMosley\ca_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="11_0FF39900EA461C03C30E4AF55D4F6E71307FC0A4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A02713C8-5FE7-46E2-BD09-78B914F50777}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09FD92C-6122-44A5-8FD5-41B5D0FBDB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19545" yWindow="0" windowWidth="15360" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30672" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Positions" sheetId="1" r:id="rId1"/>
     <sheet name="Unmatched_Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="475">
   <si>
     <t>PositionID</t>
   </si>
@@ -1444,6 +1457,9 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>E145</t>
   </si>
 </sst>
 </file>
@@ -1522,10 +1538,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1817,22 +1829,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection sqref="A1:G175"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1855,7 +1867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1878,7 +1890,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1901,7 +1913,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1924,7 +1936,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1947,7 +1959,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1970,7 +1982,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1993,7 +2005,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2016,7 +2028,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2039,7 +2051,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2062,7 +2074,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2085,7 +2097,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2108,7 +2120,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2131,7 +2143,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2177,7 +2189,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2200,7 +2212,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2223,7 +2235,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2246,7 +2258,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2269,7 +2281,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2292,7 +2304,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2315,7 +2327,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2338,7 +2350,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2361,7 +2373,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2407,7 +2419,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2430,7 +2442,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2453,7 +2465,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2476,7 +2488,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2499,7 +2511,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2522,7 +2534,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2545,7 +2557,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2568,7 +2580,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2591,7 +2603,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2614,7 +2626,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2637,7 +2649,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2660,7 +2672,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2683,7 +2695,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2706,7 +2718,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2729,7 +2741,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2752,7 +2764,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2775,7 +2787,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2798,7 +2810,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2821,7 +2833,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2844,7 +2856,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2867,7 +2879,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2890,7 +2902,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2913,7 +2925,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2936,7 +2948,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2959,7 +2971,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2982,7 +2994,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3005,7 +3017,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3028,7 +3040,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3051,7 +3063,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3074,7 +3086,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3097,12 +3109,12 @@
         <v>469</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C56">
         <v>25</v>
@@ -3111,21 +3123,21 @@
         <v>149</v>
       </c>
       <c r="E56" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="F56" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G56" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>474</v>
       </c>
       <c r="C57">
         <v>25</v>
@@ -3134,16 +3146,16 @@
         <v>156</v>
       </c>
       <c r="E57" t="s">
-        <v>167</v>
+        <v>229</v>
       </c>
       <c r="F57" t="s">
-        <v>360</v>
+        <v>265</v>
       </c>
       <c r="G57" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3166,7 +3178,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3189,7 +3201,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3212,7 +3224,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3235,7 +3247,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3258,7 +3270,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3281,7 +3293,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3304,7 +3316,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3327,7 +3339,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3350,7 +3362,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3373,7 +3385,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3396,7 +3408,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3419,7 +3431,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3442,7 +3454,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3465,7 +3477,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3488,7 +3500,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3511,7 +3523,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3534,7 +3546,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3557,7 +3569,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3580,7 +3592,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3603,7 +3615,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3626,7 +3638,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3649,7 +3661,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3672,7 +3684,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3695,7 +3707,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3718,7 +3730,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3764,7 +3776,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3787,7 +3799,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3810,7 +3822,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3833,7 +3845,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3856,7 +3868,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3879,7 +3891,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3902,7 +3914,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3925,7 +3937,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3948,7 +3960,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3971,7 +3983,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3994,7 +4006,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4017,7 +4029,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4040,7 +4052,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4063,7 +4075,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4086,7 +4098,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4109,7 +4121,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4132,7 +4144,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4155,7 +4167,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4178,7 +4190,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4201,7 +4213,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4224,7 +4236,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4247,7 +4259,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4270,7 +4282,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4293,7 +4305,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4316,7 +4328,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4339,7 +4351,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4362,7 +4374,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4385,7 +4397,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4408,7 +4420,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4431,7 +4443,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4454,7 +4466,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4477,7 +4489,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4500,7 +4512,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4523,7 +4535,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4546,7 +4558,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4569,7 +4581,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4592,7 +4604,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4615,7 +4627,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4638,7 +4650,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4661,7 +4673,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4684,7 +4696,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4707,7 +4719,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4730,7 +4742,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4753,7 +4765,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4776,7 +4788,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4799,7 +4811,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4822,7 +4834,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4845,7 +4857,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4868,7 +4880,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4891,7 +4903,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4914,7 +4926,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4937,7 +4949,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4960,7 +4972,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4983,7 +4995,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5006,7 +5018,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5029,7 +5041,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5052,7 +5064,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5075,7 +5087,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5098,7 +5110,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5121,7 +5133,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5144,7 +5156,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5167,7 +5179,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5190,7 +5202,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5213,7 +5225,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5236,7 +5248,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5259,7 +5271,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5282,7 +5294,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5305,7 +5317,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5328,7 +5340,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5351,7 +5363,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5374,7 +5386,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5397,7 +5409,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5420,7 +5432,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5443,7 +5455,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5466,7 +5478,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5489,7 +5501,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5512,7 +5524,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5535,7 +5547,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5558,7 +5570,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5581,7 +5593,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5604,7 +5616,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5627,7 +5639,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5650,7 +5662,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5673,7 +5685,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5696,7 +5708,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5719,7 +5731,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5742,7 +5754,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5765,7 +5777,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5788,7 +5800,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5811,7 +5823,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5834,7 +5846,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5858,8 +5870,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G183">
-    <sortCondition ref="C2:C183"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G175">
+    <sortCondition ref="C2:C175"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5871,9 +5883,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5890,7 +5902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5907,7 +5919,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -5924,7 +5936,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -5941,7 +5953,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -5958,7 +5970,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5975,7 +5987,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -5992,7 +6004,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -6009,7 +6021,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -6026,7 +6038,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -6043,7 +6055,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -6060,7 +6072,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -6077,7 +6089,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -6094,7 +6106,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -6111,7 +6123,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -6128,7 +6140,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -6145,7 +6157,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -6162,7 +6174,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -6179,7 +6191,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -6196,7 +6208,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>95</v>
       </c>
@@ -6213,12 +6225,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E21" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -6235,7 +6247,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -6252,7 +6264,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -6269,7 +6281,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -6286,7 +6298,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -6303,7 +6315,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -6320,7 +6332,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -6337,7 +6349,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -6354,7 +6366,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -6371,7 +6383,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -6388,7 +6400,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -6405,22 +6417,22 @@
         <v>410</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E33" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E34" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E35" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -6437,7 +6449,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -6454,7 +6466,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>122</v>
       </c>
@@ -6471,12 +6483,12 @@
         <v>415</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E39" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>123</v>
       </c>
@@ -6493,7 +6505,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -6510,7 +6522,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -6527,7 +6539,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -6544,7 +6556,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -6561,7 +6573,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -6578,7 +6590,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>141</v>
       </c>
@@ -6595,7 +6607,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -6612,12 +6624,12 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E48" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>143</v>
       </c>
@@ -6634,7 +6646,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>144</v>
       </c>
@@ -6662,9 +6674,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>429</v>
       </c>
@@ -6672,7 +6684,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>431</v>
       </c>
@@ -6680,7 +6692,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>432</v>
       </c>
@@ -6688,7 +6700,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>433</v>
       </c>

</xml_diff>